<commit_message>
Day 1/90: 5 Array Questions and 1 Linked List Question
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Algorithmic_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23792351-DE6B-49AD-8A7F-DF13F6424F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42F5405-E242-4B58-B27E-1B27241E84AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24492" yWindow="2496" windowWidth="19176" windowHeight="11220" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="22932" yWindow="1692" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1420,6 +1420,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Yes(Kadane's Algorithm)</t>
   </si>
 </sst>
 </file>
@@ -1851,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -1948,7 +1951,9 @@
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="21">
       <c r="A12" s="5" t="s">
@@ -1957,7 +1962,9 @@
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="21">
       <c r="A13" s="5" t="s">
@@ -1966,7 +1973,9 @@
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="21">
       <c r="A14" s="5" t="s">
@@ -3051,7 +3060,9 @@
       <c r="B139" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C139" s="4"/>
+      <c r="C139" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="140" spans="1:3" ht="21">
       <c r="A140" s="8" t="s">

</xml_diff>

<commit_message>
Linked 5 question solved
</commit_message>
<xml_diff>
--- a/Most-Important-Question.xlsx
+++ b/Most-Important-Question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HIGH PAYING SKILLS\Algorithmic_Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF177F41-7EEA-428A-8027-54DAE108861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBBE77-29D9-455C-8944-458131DA77B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1692" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1423,6 +1423,9 @@
   </si>
   <si>
     <t>Yes(Kadane's Algorithm)</t>
+  </si>
+  <si>
+    <t>Yes(Half)</t>
   </si>
 </sst>
 </file>
@@ -1854,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B136" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
@@ -3077,7 +3080,9 @@
       <c r="B140" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C140" s="4"/>
+      <c r="C140" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="141" spans="1:3" ht="21">
       <c r="A141" s="8" t="s">
@@ -3086,7 +3091,9 @@
       <c r="B141" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C141" s="4"/>
+      <c r="C141" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="142" spans="1:3" ht="21">
       <c r="A142" s="8" t="s">
@@ -3113,7 +3120,9 @@
       <c r="B144" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C144" s="4"/>
+      <c r="C144" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="145" spans="1:3" ht="21">
       <c r="A145" s="8" t="s">
@@ -3122,7 +3131,9 @@
       <c r="B145" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C145" s="4"/>
+      <c r="C145" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="146" spans="1:3" ht="21">
       <c r="A146" s="8" t="s">
@@ -3131,7 +3142,9 @@
       <c r="B146" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C146" s="4"/>
+      <c r="C146" s="4" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="147" spans="1:3" ht="21">
       <c r="A147" s="8" t="s">
@@ -3140,7 +3153,9 @@
       <c r="B147" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="148" spans="1:3" ht="21">
       <c r="A148" s="8" t="s">

</xml_diff>